<commit_message>
Add module post, migration, model, controller, add update row post
</commit_message>
<xml_diff>
--- a/database/seeders/Modules.xlsx
+++ b/database/seeders/Modules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="69">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -194,6 +194,39 @@
   </si>
   <si>
     <t xml:space="preserve">bi bi-check2-circle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">posts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bi bi-newspapers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">listPosts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">listPost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lista de Posts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editPost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Post</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addPost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agregar Post</t>
   </si>
 </sst>
 </file>
@@ -293,7 +326,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,6 +352,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -513,8 +550,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1063,6 +1100,195 @@
         <v>9</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add logs system, graphs with highcharts
</commit_message>
<xml_diff>
--- a/database/seeders/Modules.xlsx
+++ b/database/seeders/Modules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="79">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -242,6 +242,21 @@
   </si>
   <si>
     <t xml:space="preserve">SELECT COUNT(id) total from posts where status&gt;0 and user_id = ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graphlogs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bi bi-graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div class="row mt-4 mb-4"&gt; &lt;div class="col-md-6"&gt; &lt;div class="card mb-3"&gt; &lt;div class="card-header p-2"&gt; &lt;div class="row"&gt; &lt;div class="col-2"&gt; &lt;h5 class="card-title"&gt; &lt;i class="fa fa-bar-chart"&gt;&lt;/i&gt; Logs: &lt;/h4&gt; &lt;/div&gt; &lt;div class="col-10"&gt; &lt;div class="float-end input-group"&gt; &lt;select class="form-select form-control-sm slt-tipo-graph-logs" title="Tipo de Gráfica"&gt; &lt;option class="form-control" value="1"&gt;Barra&lt;/option&gt; &lt;option class="form-control" value="2"&gt;Lineal&lt;/option&gt; &lt;/select&gt; &lt;select class="form-select form-control-sm slt-per-graph-logs" title="Periodo"&gt; &lt;option class="form-control" value="1"&gt;Dia&lt;/option&gt; &lt;option class="form-control" value="2"&gt;Semanal&lt;/option&gt; &lt;option class="form-control" value="3"&gt;Mensual&lt;/option&gt; &lt;option class="form-control" value="4"&gt;Anual&lt;/option&gt; &lt;/select&gt; &lt;input type="date" class="form-control form-control-sm dt-per-ini-graph-logs" value="&lt;?=dayWeek('Monday');?&gt;" title="Inicio de fecha"/&gt; &lt;input type="date" class="form-control form-control-sm dt-per-fin-graph-logs" value="&lt;?=dayWeek('Saturday');?&gt;" title="Fin de fecha"/&gt; &lt;button type="button" class="btn btn-primary ml-3 btn-sm btnReloadGraph" data-graph="loadGraphLogs" title="Recargar"&gt; &lt;i class="fas fa-sync-alt"&gt;&lt;/i&gt; &lt;/button&gt; &lt;/div&gt; &lt;/div&gt; &lt;/div&gt; &lt;/div&gt; &lt;div class="card-body"&gt; &lt;div class="row div-cnt-graph-highcharts" id="div-cnt-graph-highcharts"&gt;&lt;/div&gt; &lt;/div&gt; &lt;/div&gt; &lt;script type="text/javascript"&gt; $(document).ready(function() { loadGraphLogs(); });&lt;/script&gt; &lt;/div&gt; &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -288,11 +303,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -302,6 +312,11 @@
       <name val="Liberation Mono;Courier New;DejaVu Sans Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -570,8 +585,8 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -611,7 +626,7 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -682,7 +697,7 @@
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -762,7 +777,7 @@
       <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -842,7 +857,7 @@
       <c r="E7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -922,7 +937,7 @@
       <c r="E9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1080,7 +1095,7 @@
       <c r="E13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>36</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -1118,7 +1133,7 @@
       <c r="E14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1156,7 +1171,7 @@
       <c r="E15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>61</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -1229,7 +1244,7 @@
       <c r="E17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>23</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -1268,7 +1283,7 @@
       <c r="E18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>32</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -1350,7 +1365,7 @@
       <c r="E20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>64</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -1370,6 +1385,44 @@
       </c>
       <c r="N20" s="2" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>